<commit_message>
WIP:  openpyxl-sandbox/asspy/asspy.py           |  15 ++++++++++++---  openpyxl-sandbox/{ => asspy}/example.xlsx | Bin  openpyxl-sandbox/asspy/new.xlsx           | Bin 5550 -> 5420 bytes  openpyxl-sandbox/asspy/template.xlsx      | Bin 5550 -> 5699 bytes  4 files changed, 12 insertions(+), 3 deletions(-)
</commit_message>
<xml_diff>
--- a/openpyxl-sandbox/asspy/template.xlsx
+++ b/openpyxl-sandbox/asspy/template.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet!$A$1:$C$2</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -227,10 +230,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -260,6 +263,39 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>